<commit_message>
Final draft (no quotes)
</commit_message>
<xml_diff>
--- a/chalice2sil/doc/report/benchmark.xlsx
+++ b/chalice2sil/doc/report/benchmark.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Pivot-2" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Data!$A$1:$AN$88</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Data-present'!$A$1:$I$86</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="39" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="178">
   <si>
     <t>ToSIL-1</t>
   </si>
@@ -554,6 +555,21 @@
   <si>
     <t>Syxc</t>
   </si>
+  <si>
+    <t>exception in Chalice2SIL during translation of expression involving 'waitlevel'</t>
+  </si>
+  <si>
+    <t>exception in Chalice2SIL during resolution of a field name</t>
+  </si>
+  <si>
+    <t>exception in Chalice2SIL during translation of a type expression</t>
+  </si>
+  <si>
+    <t>exception in Chalice2SIL during substitution of program variables</t>
+  </si>
+  <si>
+    <t>channels not supported by Chalice2SIL</t>
+  </si>
 </sst>
 </file>
 
@@ -828,10 +844,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -839,148 +852,13 @@
       <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0\ &quot;ms&quot;"/>
+      <numFmt numFmtId="169" formatCode="0\ &quot;ms&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0\ &quot;ms&quot;"/>
@@ -1716,11 +1594,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="643052176"/>
-        <c:axId val="415240856"/>
+        <c:axId val="483939480"/>
+        <c:axId val="483941832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="643052176"/>
+        <c:axId val="483939480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,7 +1643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415240856"/>
+        <c:crossAx val="483941832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1773,7 +1651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="415240856"/>
+        <c:axId val="483941832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1835,7 +1713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="643052176"/>
+        <c:crossAx val="483939480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1849,7 +1727,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6269,7 +6146,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="39">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="39">
   <location ref="A9:D21" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="7" colPageCount="1"/>
   <pivotFields count="39">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -6539,13 +6416,13 @@
     <dataField name="Silicon" fld="23" subtotal="average" baseField="1" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="36">
+    <format dxfId="5">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="55">
@@ -6608,7 +6485,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="22">
@@ -6732,7 +6609,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="23">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="23">
   <location ref="A8:B17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="5" colPageCount="1"/>
   <pivotFields count="39">
     <pivotField showAll="0"/>
@@ -6878,10 +6755,10 @@
     <dataField name="Count of comment" fld="18" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="50">
+    <format dxfId="1">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -7597,10 +7474,10 @@
   <dimension ref="A1:AN228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG45" sqref="AG45"/>
+      <selection pane="bottomRight" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7619,7 +7496,7 @@
     <col min="15" max="15" width="7.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="71.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.5703125" style="27" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5703125" style="27" customWidth="1"/>
     <col min="22" max="22" width="10.85546875" style="3" customWidth="1"/>
@@ -11765,7 +11642,7 @@
       </c>
       <c r="R31" s="20"/>
       <c r="S31" s="15" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="T31" s="20">
         <f t="shared" si="10"/>
@@ -12303,7 +12180,7 @@
       </c>
       <c r="R35" s="20"/>
       <c r="S35" s="15" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="T35" s="20">
         <f t="shared" si="10"/>
@@ -14115,7 +13992,7 @@
       </c>
       <c r="R48" s="20"/>
       <c r="S48" s="15" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="T48" s="20">
         <f t="shared" si="10"/>
@@ -14371,7 +14248,7 @@
       </c>
       <c r="R50" s="20"/>
       <c r="S50" s="15" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="T50" s="20">
         <f t="shared" si="10"/>
@@ -16161,7 +16038,7 @@
       </c>
       <c r="R64" s="20"/>
       <c r="S64" s="15" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="T64" s="20">
         <f t="shared" si="10"/>
@@ -17637,7 +17514,7 @@
       </c>
       <c r="R76" s="20"/>
       <c r="S76" s="15" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
       <c r="T76" s="20">
         <f t="shared" si="37"/>
@@ -18031,7 +17908,7 @@
       </c>
       <c r="R79" s="20"/>
       <c r="S79" s="15" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="T79" s="20">
         <f t="shared" si="37"/>
@@ -18143,7 +18020,7 @@
       </c>
       <c r="R80" s="20"/>
       <c r="S80" s="15" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
       <c r="T80" s="20">
         <f t="shared" si="37"/>
@@ -18255,7 +18132,7 @@
       </c>
       <c r="R81" s="20"/>
       <c r="S81" s="15" t="s">
-        <v>67</v>
+        <v>176</v>
       </c>
       <c r="T81" s="20">
         <f t="shared" si="37"/>
@@ -18764,7 +18641,7 @@
       </c>
       <c r="R85" s="20"/>
       <c r="S85" s="15" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="T85" s="20">
         <f t="shared" si="37"/>
@@ -19966,6 +19843,7 @@
       <c r="S228" s="27"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AN88"/>
   <conditionalFormatting sqref="Q60:Q71">
     <cfRule type="colorScale" priority="9">
       <colorScale>

</xml_diff>